<commit_message>
timesheet & camunda controller part
</commit_message>
<xml_diff>
--- a/Naveenraj/TimeSheet/Schwall_Naveenraj_Timesheet_November_2021.xlsx
+++ b/Naveenraj/TimeSheet/Schwall_Naveenraj_Timesheet_November_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schwall_Camunda_GITHUB\JavaTraining-Batch1\Naveenraj\TimeSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DDDAC0-DE1E-457B-9723-9D2CC9EAF621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8368689D-3ECB-45DC-A413-CD86ED2BB517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{23EAE99D-3C5B-4F90-9213-F90EE225C610}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>SCHWALL WEEKLY TIMESHEET</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>Create Table in DB / h2</t>
+  </si>
+  <si>
+    <t>Start Instance in runtime</t>
   </si>
 </sst>
 </file>
@@ -263,6 +266,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -272,10 +279,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,7 +596,7 @@
   <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -606,13 +609,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -632,718 +635,726 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="5">
         <v>44501</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="5">
         <v>44502</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="5">
         <v>44503</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="5">
         <v>44504</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="5">
         <v>44505</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="5">
         <v>44508</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="5">
         <v>44509</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="5">
         <v>44510</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="7">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="5">
         <v>44511</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="5">
         <v>44512</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="5">
         <v>44515</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="5">
         <v>44517</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="5">
         <v>44518</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="5">
         <v>44519</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="5">
         <v>44522</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
+      <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
+      <c r="B18" s="5">
+        <v>44523</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="7">
+        <v>6</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
+      <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="7">
+      <c r="A20" s="4">
         <v>18</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
+      <c r="A21" s="4">
         <v>19</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
+      <c r="A22" s="4">
         <v>20</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="10"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
+      <c r="A23" s="4">
         <v>21</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="10"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
+      <c r="A24" s="4">
         <v>22</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="10"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="7">
+      <c r="A25" s="4">
         <v>23</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="10"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="7">
+      <c r="A26" s="4">
         <v>24</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="7">
+      <c r="A27" s="4">
         <v>25</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="10"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="7">
+      <c r="A28" s="4">
         <v>26</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="10"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="7">
+      <c r="A29" s="4">
         <v>27</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="10"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="7">
+      <c r="A30" s="4">
         <v>28</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="10"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="7">
+      <c r="A31" s="4">
         <v>29</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="10"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="7">
+      <c r="A32" s="4">
         <v>30</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="10"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="7">
+      <c r="A33" s="4">
         <v>31</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="10"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="7">
+      <c r="A34" s="4">
         <v>32</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="10"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="7">
+      <c r="A35" s="4">
         <v>33</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="10"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="7">
+      <c r="A36" s="4">
         <v>34</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="10"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="7">
+      <c r="A37" s="4">
         <v>35</v>
       </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="10"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="7">
+      <c r="A38" s="4">
         <v>36</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="10"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="7">
+      <c r="A39" s="4">
         <v>37</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="10"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="7">
+      <c r="A40" s="4">
         <v>38</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="10"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="7">
+      <c r="A41" s="4">
         <v>39</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="10"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="7">
+      <c r="A42" s="4">
         <v>40</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="10"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="7">
+      <c r="A43" s="4">
         <v>41</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="10"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="7">
+      <c r="A44" s="4">
         <v>42</v>
       </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="10"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="7"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="7">
+      <c r="A45" s="4">
         <v>43</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="10"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="7">
+      <c r="A46" s="4">
         <v>44</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="10"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="7">
+      <c r="A47" s="4">
         <v>45</v>
       </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="10"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="7"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="7">
+      <c r="A48" s="4">
         <v>46</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="10"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="7">
+      <c r="A49" s="4">
         <v>47</v>
       </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="10"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="7"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="7">
+      <c r="A50" s="4">
         <v>48</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="10"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="7">
+      <c r="A51" s="4">
         <v>49</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="10"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="7">
+      <c r="A52" s="4">
         <v>50</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="10"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="7"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="7">
+      <c r="A53" s="4">
         <v>51</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="10"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="7">
+      <c r="A54" s="4">
         <v>52</v>
       </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="10"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="7">
+      <c r="A55" s="4">
         <v>53</v>
       </c>
-      <c r="B55" s="8"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="10"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="7">
+      <c r="A56" s="4">
         <v>54</v>
       </c>
-      <c r="B56" s="8"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="10"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="7"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="7">
+      <c r="A57" s="4">
         <v>55</v>
       </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="10"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="7"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="7">
+      <c r="A58" s="4">
         <v>56</v>
       </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="10"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="7"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="7">
+      <c r="A59" s="4">
         <v>57</v>
       </c>
-      <c r="B59" s="8"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="10"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="7"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="7">
+      <c r="A60" s="4">
         <v>58</v>
       </c>
-      <c r="B60" s="8"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="10"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="7"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="7">
+      <c r="A61" s="4">
         <v>59</v>
       </c>
-      <c r="B61" s="8"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="10"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="7"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="7">
+      <c r="A62" s="4">
         <v>60</v>
       </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="10"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="7"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="7">
+      <c r="A63" s="4">
         <v>61</v>
       </c>
-      <c r="B63" s="8"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="10"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="7"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="7">
+      <c r="A64" s="4">
         <v>62</v>
       </c>
-      <c r="B64" s="8"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="10"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="7"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="7">
+      <c r="A65" s="4">
         <v>63</v>
       </c>
-      <c r="B65" s="8"/>
-      <c r="C65" s="9"/>
-      <c r="D65" s="9"/>
-      <c r="E65" s="10"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="7"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="7">
+      <c r="A66" s="4">
         <v>64</v>
       </c>
-      <c r="B66" s="8"/>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="10"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="7"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="7">
+      <c r="A67" s="4">
         <v>65</v>
       </c>
-      <c r="B67" s="8"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="10"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="7"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="7">
+      <c r="A68" s="4">
         <v>66</v>
       </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="10"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>